<commit_message>
Return and Exchanges latest updates
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="511">
   <si>
     <t>Ankit</t>
   </si>
@@ -5491,7 +5491,7 @@
       <c r="CE33" s="1"/>
       <c r="CF33" s="18"/>
       <c r="CG33" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:85" x14ac:dyDescent="0.25">
@@ -11888,7 +11888,7 @@
       <c r="CE97" s="30"/>
       <c r="CF97" s="30"/>
       <c r="CG97" s="29" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" ht="30" r="98" s="29" spans="1:85" x14ac:dyDescent="0.25">
@@ -11991,7 +11991,7 @@
       <c r="CE98" s="30"/>
       <c r="CF98" s="30"/>
       <c r="CG98" s="29" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row customFormat="1" ht="30" r="99" s="29" spans="1:85" x14ac:dyDescent="0.25">

</xml_diff>